<commit_message>
Changes in config.json and function names
</commit_message>
<xml_diff>
--- a/final_output/0270-049-ENOD.labeled_final_results.xlsx
+++ b/final_output/0270-049-ENOD.labeled_final_results.xlsx
@@ -1,14 +1,32 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PR results" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -19,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -27,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -390,4 +417,249 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IntervarClassification</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarClinicalSignificance</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ReviewStatus</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarID</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Orpha</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Phenotype</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ACMG_version</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>OMIM_disorder</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>inheritance</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>variants_to_report</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>related_HPOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2:48030640:C:-</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MSH6</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>rs267608078</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>144|-|Unknown|Autosomal dominant|Adult|120435 609310 613244 614331 614337 614350 614385 ~252202|CMMR-D syndrome|-|Autosomal recessive|Childhood|276300 ~</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Lynch syndrome (HNPCC)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>614350</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>All P and LP</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2:179456907:A:-</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TTN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Likely pathogenic</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>289377|-|Unknown|Autosomal recessive|Childhood|611705 ~140922|LGMD2J|&lt;1 / 1 000 000|-|Childhood&lt;br&gt;Adolescent&lt;br&gt;Adult|608807 ~154|Familial or idiopathic dilated cardiomyopathy|1-5 / 10 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Mitochondrial inheritance|All ages|302045 600884 601154 601493 601494 604145 604288 604765 605582 606685 607482 608569 609909 609915 611407 611615 611878 611879 611880 612158 612877 613122 613172 613252 613286 613424 613426 613642 613694 613697 613740 613881 614672 615184 615235 615248 615373 615396 615916 ~178464|ADMERF&lt;br&gt;Edström Myopathy&lt;br&gt;HIBM-ERF&lt;br&gt;HMERF&lt;br&gt;Hereditary inclusion body myopathy with early respiratory failure&lt;br&gt;Myofibrillar myopathy with early respiratory failure|&lt;1 / 1 000 000|Autosomal dominant|-|603689 ~609|Distal myopathy, Udd type&lt;br&gt;Distal titinopathy&lt;br&gt;Finnish tibial muscular dystrophy&lt;br&gt;TMD&lt;br&gt;Udd myopathy|1-9 / 100 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Adult|600334 ~</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Dilated cardiomyopathy</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>604145</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>All P and LP. Only loss-of-function variants should be reported as a secondary finding.</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modifications in PR module execution
</commit_message>
<xml_diff>
--- a/final_output/0270-049-ENOD.labeled_final_results.xlsx
+++ b/final_output/0270-049-ENOD.labeled_final_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,55 +451,60 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>IntervarConsequence</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>IntervarClassification</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ClinvarClinicalSignificance</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ReviewStatus</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ClinvarID</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Orpha</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Phenotype</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>ACMG_version</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>OMIM_disorder</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>inheritance</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>variants_to_report</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>related_HPOs</t>
         </is>
@@ -528,55 +533,60 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>exonic,frameshift deletion</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Pathogenic</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>144|-|Unknown|Autosomal dominant|Adult|120435 609310 613244 614331 614337 614350 614385 ~252202|CMMR-D syndrome|-|Autosomal recessive|Childhood|276300 ~</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Lynch syndrome (HNPCC)</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>614350</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>AD</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>All P and LP</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
@@ -605,55 +615,60 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>exonic,frameshift deletion</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Likely pathogenic</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>289377|-|Unknown|Autosomal recessive|Childhood|611705 ~140922|LGMD2J|&lt;1 / 1 000 000|-|Childhood&lt;br&gt;Adolescent&lt;br&gt;Adult|608807 ~154|Familial or idiopathic dilated cardiomyopathy|1-5 / 10 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Mitochondrial inheritance|All ages|302045 600884 601154 601493 601494 604145 604288 604765 605582 606685 607482 608569 609909 609915 611407 611615 611878 611879 611880 612158 612877 613122 613172 613252 613286 613424 613426 613642 613694 613697 613740 613881 614672 615184 615235 615248 615373 615396 615916 ~178464|ADMERF&lt;br&gt;Edström Myopathy&lt;br&gt;HIBM-ERF&lt;br&gt;HMERF&lt;br&gt;Hereditary inclusion body myopathy with early respiratory failure&lt;br&gt;Myofibrillar myopathy with early respiratory failure|&lt;1 / 1 000 000|Autosomal dominant|-|603689 ~609|Distal myopathy, Udd type&lt;br&gt;Distal titinopathy&lt;br&gt;Finnish tibial muscular dystrophy&lt;br&gt;TMD&lt;br&gt;Udd myopathy|1-9 / 100 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Adult|600334 ~</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Dilated cardiomyopathy</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>604145</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>AD</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>All P and LP. Only loss-of-function variants should be reported as a secondary finding.</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>NA</t>
         </is>

</xml_diff>

<commit_message>
Common functions placed to utils.py file. RR module changanges
</commit_message>
<xml_diff>
--- a/final_output/0270-049-ENOD.labeled_final_results.xlsx
+++ b/final_output/0270-049-ENOD.labeled_final_results.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PR results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RR results" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -513,7 +514,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2:48030640:C:-</t>
+          <t>2:48030639:AC:A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -543,17 +544,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pathogenic</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(3) reviewed by expert panel</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>RCV000009499|RCV000074830|RCV000115411|RCV000202045|RCV000524165|RCV001353984|RCV001249957|RCV001824596|RCV001762178|RCV002498358|RCV003162476</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -595,7 +596,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2:179456907:A:-</t>
+          <t>2:179456906:TA:T</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -610,7 +611,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -625,50 +626,664 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>289377|-|Unknown|Autosomal recessive|Childhood|611705 ~140922|LGMD2J|&lt;1 / 1 000 000|-|Childhood&lt;br&gt;Adolescent&lt;br&gt;Adult|608807 ~154|Familial or idiopathic dilated cardiomyopathy|1-5 / 10 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Mitochondrial inheritance|All ages|302045 600884 601154 601493 601494 604145 604288 604765 605582 606685 607482 608569 609909 609915 611407 611615 611878 611879 611880 612158 612877 613122 613172 613252 613286 613424 613426 613642 613694 613697 613740 613881 614672 615184 615235 615248 615373 615396 615916 ~178464|ADMERF&lt;br&gt;Edström Myopathy&lt;br&gt;HIBM-ERF&lt;br&gt;HMERF&lt;br&gt;Hereditary inclusion body myopathy with early respiratory failure&lt;br&gt;Myofibrillar myopathy with early respiratory failure|&lt;1 / 1 000 000|Autosomal dominant|-|603689 ~609|Distal myopathy, Udd type&lt;br&gt;Distal titinopathy&lt;br&gt;Finnish tibial muscular dystrophy&lt;br&gt;TMD&lt;br&gt;Udd myopathy|1-9 / 100 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Adult|600334 ~</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Dilated cardiomyopathy</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>604145</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>All P and LP. Only loss-of-function variants should be reported as a secondary finding.</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IntervarConsequence</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>IntervarClassification</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarClinicalSignificance</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ReviewStatus</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarID</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Orpha</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Phenotype</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ACMG_version</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OMIM_disorder</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>inheritance</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>variants_to_report</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>related_HPOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>1:216370044:G:A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>USH2A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>rs755867377</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Conflicting interpretations of pathogenicity</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>(1) criteria provided, conflicting interpretations</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>RCV001074212|RCV002554704</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>791|-|1-5 / 10 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Mitochondrial inheritance|Childhood&lt;br&gt;Adolescent&lt;br&gt;Adult|180100 180104 180105 180210 268000 268025 268060 300029 300155 300424 300605 312600 312612 400004 600059 600105 600132 600138 600852 601414 601718 602594 602772 604232 604393 606068 607921 608133 608380 609913 609923 610282 610359 610599 611131 612095 612165 612572 612712 612943 613194 613341 613428 613464 613575 613581 613582 613617 613660 613731 613750 613756 613758 613767 613769 613794 613801 613809 613810 613827 613861 613862 613983 614180 614181 614494 614500 615233 615434 615565 615725 615780 615922 616188 616394 616469 616544 616562 617023 617123 ~231178|USH2|1-9 / 100 000|Autosomal recessive|Infancy&lt;br&gt;Childhood&lt;br&gt;Adolescent|276901 605472 611383 ~886|Retinitis pigmentosa-deafness syndrome&lt;br&gt;USH|1-9 / 100 000|Autosomal recessive|Infancy&lt;br&gt;Neonatal|276900 276901 276902 276904 500004 601067 602083 602097 605472 606943 611383 612632 614504 614869 614990 ~</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Usher syndrome, type 2A</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>276901</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>7:107329557:T:C</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SLC26A4</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>rs111033243</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Conflicting interpretations of pathogenicity</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>(1) criteria provided, conflicting interpretations</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>RCV000036423|RCV000756644|RCV000987940|RCV001004634</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>90636|Autosomal recessive isolated neurosensory deafness type DFNB&lt;br&gt;Autosomal recessive isolated sensorineural deafness type DFNB&lt;br&gt;Autosomal recessive non-syndromic neurosensory deafness type DFNB|Unknown|Autosomal recessive|Infancy&lt;br&gt;Neonatal|220290 600060 600316 600791 600792 600971 600974 601071 601072 601386 601869 602092 603010 603098 603629 603678 603720 604060 605428 605818 607039 607084 607101 607239 607821 608219 608264 608265 608565 608653 609006 609439 609533 609646 609647 609706 609823 609941 609946 609952 610143 610153 610154 610212 610220 610248 610265 610419 611022 611451 612433 612645 612789 613079 613285 613307 613391 613392 613453 613685 613718 613865 613916 614035 614414 614617 614861 614899 614934 614944 614945 615429 615540 615837 615974 616042 616515 616705 616958 ~705|Goiter-deafness syndrome|1-9 / 100 000|Autosomal recessive|Infancy&lt;br&gt;Neonatal|274600 ~</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Deafness autosomal recessive 4; Pendred syndrome</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>600791; 274600</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>7:117199644:ATCT:A</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CFTR</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>rs113993960</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>exonic,nonframeshift deletion</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>(4) practice guideline</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>RCV000007523|RCV000007524|RCV000058929|RCV000119038|RCV000624683|RCV000626692|RCV000626693|RCV001004459|RCV001642198|RCV001831519|RCV001787371|RCV001787370|RCV002251888|RCV002243627|RCV002490332|RCV003227599|RCV003398459|RCV003444054</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>48|Congenital bilateral agenesis of vas deferens&lt;br&gt;Congenital bilateral aplasia of vas deferens|1-5 / 10 000|X-linked recessive&lt;br&gt;or&amp;nbsp;Autosomal recessive|Adolescent&lt;br&gt;Adult|277180 300985 ~586|CF&lt;br&gt;Mucoviscidosis|1-9 / 100 000|Autosomal recessive|All ages|219700 ~60033|-|-|-|-|211400 613021 613071 ~676|-|1-9 / 1 000 000|Autosomal dominant|Childhood&lt;br&gt;Adolescent|167800 ~</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Cystic fibrosis</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>219700</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>11:17496515:C:T</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ABCC8</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>rs764349043</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Conflicting interpretations of pathogenicity</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>(1) criteria provided, conflicting interpretations</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>RCV002224395|RCV002487022|RCV003418409</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>99886|TNDM|Unknown|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;Not applicable|Antenatal&lt;br&gt;Neonatal|601410 610374 610582 ~79134|Developmental delay-epilepsy-neonatal diabetes syndrome|&lt;1 / 1 000 000|Not applicable&lt;br&gt;or&amp;nbsp;Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Infancy&lt;br&gt;Neonatal|606176 ~99885|Monogenic diabetes of infancy&lt;br&gt;PNDM|1-9 / 1 000 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Antenatal&lt;br&gt;Neonatal&lt;br&gt;Infancy|606176 ~276575|Autosomal dominant hyperinsulinemic hypoglycemia due to SUR1 deficiency|Unknown|Autosomal dominant|Infancy&lt;br&gt;Neonatal|256450 ~276598|Hyperinsulinemic hypoglycemia due to SUR1 deficiency, diazoxide-resistant focal form|Unknown|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Infancy&lt;br&gt;Neonatal|256450 ~79643|Autosomal recessive hyperinsulinemic hypoglycemia due to SUR1 deficiency|-|Autosomal recessive|-|256450 ~</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Diabetes mellitus, permanent neonatal 3</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>618857</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>12:103306572:A:C</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PAH</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>rs199475598</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Likely pathogenic</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pathogenic/Likely pathogenic</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>(2) criteria provided, multiple submitters, no conflicts</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>RCV000078512|RCV000150092|RCV000588067|RCV002251964</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2209|Hyperphenylalaninemic embryopathy&lt;br&gt;Maternal PKU&lt;br&gt;Maternal hyperphenylalaninemia&lt;br&gt;Phenylketonuric embryopathy|Unknown|Autosomal recessive|Neonatal&lt;br&gt;Antenatal|261600 ~716|PAH deficiency&lt;br&gt;PKU&lt;br&gt;Phenylalanine hydroxylase deficiency|1-5 / 10 000|Autosomal recessive|Infancy|261600 ~</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Phenylketonuria</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>261600</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>15:91304138:GA:G</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BLM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>rs772495493</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>exonic,frameshift deletion</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>(2) criteria provided, multiple submitters, no conflicts</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>RCV000415444|RCV002402108|RCV003321587</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>125|BSyn|Unknown|Autosomal recessive|Neonatal&lt;br&gt;Antenatal|210900 ~</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Bloom syndrome</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>210900</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>X:25031367:C:A</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ARX</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>289377|-|Unknown|Autosomal recessive|Childhood|611705 ~140922|LGMD2J|&lt;1 / 1 000 000|-|Childhood&lt;br&gt;Adolescent&lt;br&gt;Adult|608807 ~154|Familial or idiopathic dilated cardiomyopathy|1-5 / 10 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Mitochondrial inheritance|All ages|302045 600884 601154 601493 601494 604145 604288 604765 605582 606685 607482 608569 609909 609915 611407 611615 611878 611879 611880 612158 612877 613122 613172 613252 613286 613424 613426 613642 613694 613697 613740 613881 614672 615184 615235 615248 615373 615396 615916 ~178464|ADMERF&lt;br&gt;Edström Myopathy&lt;br&gt;HIBM-ERF&lt;br&gt;HMERF&lt;br&gt;Hereditary inclusion body myopathy with early respiratory failure&lt;br&gt;Myofibrillar myopathy with early respiratory failure|&lt;1 / 1 000 000|Autosomal dominant|-|603689 ~609|Distal myopathy, Udd type&lt;br&gt;Distal titinopathy&lt;br&gt;Finnish tibial muscular dystrophy&lt;br&gt;TMD&lt;br&gt;Udd myopathy|1-9 / 100 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Adult|600334 ~</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Dilated cardiomyopathy</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>604145</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>AD</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>All P and LP. Only loss-of-function variants should be reported as a secondary finding.</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>exonic,stopgain</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>94083|Partington-Mulley syndrome&lt;br&gt;X-linked intellectual disability-dystonia-dysarthria syndrome|&lt;1 / 1 000 000|X-linked recessive|Childhood|309510 ~1934|EIEE&lt;br&gt;Early infantile epileptic encephalopathy with suppression-bursts&lt;br&gt;Ohtahara syndrome|Unknown|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Not applicable|Neonatal|300672 308350 609304 612164 613402 613721 615473 616341 ~3175|-|&lt;1 / 1 000 000|X-linked recessive|No data available|308350 ~3451|Infantile spasms&lt;br&gt;Intellectual disability-hypsarrhythmia syndrome|1-9 / 100 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive|Infancy&lt;br&gt;Neonatal&lt;br&gt;Childhood|300672 308350 613477 613722 615006 616139 616341 617065 ~364063|-|-|X-linked recessive|Infancy&lt;br&gt;Neonatal|308350 ~777|X-linked non-specific intellectual disability|Unknown|X-linked recessive|Childhood|300046 300047 300062 300114 300115 300143 300210 300271 300324 300355 300372 300387 300419 300428 300433 300436 300454 300498 300504 300505 300518 300558 300705 300716 300802 300803 300844 300848 300849 300850 300851 300852 300919 300928 300978 300983 300984 309530 309549 ~452|X-linked lissencephaly with ambiguous genitalia&lt;br&gt;X-linked lissencephaly-agenesis of the corpus callosum-genital anomalies syndrome&lt;br&gt;XLAG (X-linked lissencephaly with abnormal genitalia) syndrome|Unknown|X-linked recessive|Neonatal|300215 ~2508|Proud-Levine-Carpenter syndrome|Unknown|X-linked recessive|Infancy&lt;br&gt;Neonatal|300004 ~</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Developmental and epileptic encephalopathy 1 (DEE1)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>308350</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
         <is>
           <t>NA</t>
         </is>

</xml_diff>

<commit_message>
clinvarID is used as an identifier from Clinvar DDBB
</commit_message>
<xml_diff>
--- a/final_output/0270-049-ENOD.labeled_final_results.xlsx
+++ b/final_output/0270-049-ENOD.labeled_final_results.xlsx
@@ -554,7 +554,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>RCV000009499|RCV000074830|RCV000115411|RCV000202045|RCV000524165|RCV001353984|RCV001249957|RCV001824596|RCV001762178|RCV002498358|RCV003162476</t>
+          <t>89363</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>RCV001074212|RCV002554704</t>
+          <t>866323</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>RCV000036423|RCV000756644|RCV000987940|RCV001004634</t>
+          <t>43492</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -962,7 +962,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>RCV000007523|RCV000007524|RCV000058929|RCV000119038|RCV000624683|RCV000626692|RCV000626693|RCV001004459|RCV001642198|RCV001831519|RCV001787371|RCV001787370|RCV002251888|RCV002243627|RCV002490332|RCV003227599|RCV003398459|RCV003444054</t>
+          <t>7105</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>RCV002224395|RCV002487022|RCV003418409</t>
+          <t>1677653</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>RCV000078512|RCV000150092|RCV000588067|RCV002251964</t>
+          <t>92734</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>RCV000415444|RCV002402108|RCV003321587</t>
+          <t>374315</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">

</xml_diff>

<commit_message>
Get versions and paths for dependencies and files and save them into the final report
</commit_message>
<xml_diff>
--- a/final_output/0270-049-ENOD.labeled_final_results.xlsx
+++ b/final_output/0270-049-ENOD.labeled_final_results.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FG results" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FG Diplotype-Phenotype" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Versions and Paths&quot;" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FG results" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FG Diplotype-Phenotype" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,198 +438,204 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Variant</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GT</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>rs</t>
+          <t>SF module</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0.1</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2:234665659:T:G</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>SF module mode</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1/1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>UGT1A1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>rs4124874</t>
+          <t>advanced</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>7:99361466:C:T</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Input VCF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0/1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CYP3A4</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>rs2242480</t>
+          <t>/home/jpflorido/GBPA/projects/secondaryfindings/examples/0270-049-ENOD.labeled.vcf.gz</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>12:21329738:A:G</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Temporal dir</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0/1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>SLCO1B1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>rs2306283</t>
+          <t>/home/jpflorido/GBPA/projects/secondaryfindings/temp/</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>12:21331549:T:C</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Output dir</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0/1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>SLCO1B1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>rs4149056</t>
+          <t>/home/jpflorido/GBPA/projects/secondaryfindings/final_output/</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>16:31104878:G:A</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>HPO list</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0/1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>VKORC1</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>rs9934438</t>
+          <t>Not provided</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>16:31107689:C:T</t>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Human assembly</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0/1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>VKORC1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>rs9923231</t>
+          <t>hg19</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>19:41512841:G:T</t>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Reference genome path</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0/1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CYP2B6</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>rs3745274</t>
+          <t>/mnt/lustre/scratch/CBRA/data/indexed_genomes/bwa/hs37d5/hs37d5.fa</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>22:42526763:C:T</t>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Clinvar version</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0/1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>rs769258</t>
+          <t>20240107</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Clinvar path</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>/home/jpflorido/software/clinvar/clinvar_database_GRCh37_20240107.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Clinvar Evidence level</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Intervar version</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2.2.2 20210727</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Intervar path</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>/home/jpflorido/software/InterVar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>bcftools version</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>bcftools path</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>/home/jpflorido/software/bcftools-1.16/</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>HPO genes to phenotype version</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16012024</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>HPO genes to phenotype path</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>/home/jpflorido/GBPA/projects/secondaryfindings/categories/hpo_genes_to_phenotype_16012024.txt</t>
         </is>
       </c>
     </row>
@@ -643,147 +650,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gene</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Diplotipo</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Phenotype</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Activity Score</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CYP2C9</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>*1/*1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Normal Metabolizer</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CYP2C19</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>*1/*1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Normal Metabolizer</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DPYD</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>*1/*1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Normal Metabolizer</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>NUDT15</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>*1/*1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Normal Metabolizer</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>TPMT</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>*1/*1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Normal Metabolizer</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
VCF header is included when intersecting with BED
</commit_message>
<xml_diff>
--- a/final_output/0270-049-ENOD.labeled_final_results.xlsx
+++ b/final_output/0270-049-ENOD.labeled_final_results.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Versions and Paths&quot;" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FG results" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FG Diplotype-Phenotype" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Versions and Paths" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PR results" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RR results" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -650,14 +650,256 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IntervarConsequence</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>IntervarClassification</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarClinicalSignificance</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ReviewStatus</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarID</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Orpha</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Phenotype</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ACMG_version</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OMIM_disorder</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>inheritance</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>variants_to_report</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>related_HPOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2:48030639:AC:A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MSH6</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>rs267608078</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>exonic,frameshift deletion</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>(3) reviewed by expert panel</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>89363</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>144|-|Unknown|Autosomal dominant|Adult|120435 609310 613244 614331 614337 614350 614385 ~252202|CMMR-D syndrome|-|Autosomal recessive|Childhood|276300 ~</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Lynch syndrome (HNPCC)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>614350</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>All P and LP</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2:179456906:TA:T</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TTN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>exonic,frameshift deletion</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Likely pathogenic</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>289377|-|Unknown|Autosomal recessive|Childhood|611705 ~140922|LGMD2J|&lt;1 / 1 000 000|-|Childhood&lt;br&gt;Adolescent&lt;br&gt;Adult|608807 ~154|Familial or idiopathic dilated cardiomyopathy|1-5 / 10 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Mitochondrial inheritance|All ages|302045 600884 601154 601493 601494 604145 604288 604765 605582 606685 607482 608569 609909 609915 611407 611615 611878 611879 611880 612158 612877 613122 613172 613252 613286 613424 613426 613642 613694 613697 613740 613881 614672 615184 615235 615248 615373 615396 615916 ~178464|ADMERF&lt;br&gt;Edström Myopathy&lt;br&gt;HIBM-ERF&lt;br&gt;HMERF&lt;br&gt;Hereditary inclusion body myopathy with early respiratory failure&lt;br&gt;Myofibrillar myopathy with early respiratory failure|&lt;1 / 1 000 000|Autosomal dominant|-|603689 ~609|Distal myopathy, Udd type&lt;br&gt;Distal titinopathy&lt;br&gt;Finnish tibial muscular dystrophy&lt;br&gt;TMD&lt;br&gt;Udd myopathy|1-9 / 100 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Adult|600334 ~</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Dilated cardiomyopathy</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>604145</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>All P and LP. Only loss-of-function variants should be reported as a secondary finding.</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -668,14 +910,610 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Gene</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IntervarConsequence</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>IntervarClassification</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarClinicalSignificance</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ReviewStatus</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ClinvarID</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Orpha</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Phenotype</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ACMG_version</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OMIM_disorder</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>inheritance</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>variants_to_report</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>related_HPOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>1:216370044:G:A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>USH2A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>rs755867377</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Conflicting interpretations of pathogenicity</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>(1) criteria provided, conflicting interpretations</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>866323</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>791|-|1-5 / 10 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Mitochondrial inheritance|Childhood&lt;br&gt;Adolescent&lt;br&gt;Adult|180100 180104 180105 180210 268000 268025 268060 300029 300155 300424 300605 312600 312612 400004 600059 600105 600132 600138 600852 601414 601718 602594 602772 604232 604393 606068 607921 608133 608380 609913 609923 610282 610359 610599 611131 612095 612165 612572 612712 612943 613194 613341 613428 613464 613575 613581 613582 613617 613660 613731 613750 613756 613758 613767 613769 613794 613801 613809 613810 613827 613861 613862 613983 614180 614181 614494 614500 615233 615434 615565 615725 615780 615922 616188 616394 616469 616544 616562 617023 617123 ~231178|USH2|1-9 / 100 000|Autosomal recessive|Infancy&lt;br&gt;Childhood&lt;br&gt;Adolescent|276901 605472 611383 ~886|Retinitis pigmentosa-deafness syndrome&lt;br&gt;USH|1-9 / 100 000|Autosomal recessive|Infancy&lt;br&gt;Neonatal|276900 276901 276902 276904 500004 601067 602083 602097 605472 606943 611383 612632 614504 614869 614990 ~</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Usher syndrome, type 2A</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>276901</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>7:107329557:T:C</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SLC26A4</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>rs111033243</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Conflicting interpretations of pathogenicity</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>(1) criteria provided, conflicting interpretations</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>43492</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>90636|Autosomal recessive isolated neurosensory deafness type DFNB&lt;br&gt;Autosomal recessive isolated sensorineural deafness type DFNB&lt;br&gt;Autosomal recessive non-syndromic neurosensory deafness type DFNB|Unknown|Autosomal recessive|Infancy&lt;br&gt;Neonatal|220290 600060 600316 600791 600792 600971 600974 601071 601072 601386 601869 602092 603010 603098 603629 603678 603720 604060 605428 605818 607039 607084 607101 607239 607821 608219 608264 608265 608565 608653 609006 609439 609533 609646 609647 609706 609823 609941 609946 609952 610143 610153 610154 610212 610220 610248 610265 610419 611022 611451 612433 612645 612789 613079 613285 613307 613391 613392 613453 613685 613718 613865 613916 614035 614414 614617 614861 614899 614934 614944 614945 615429 615540 615837 615974 616042 616515 616705 616958 ~705|Goiter-deafness syndrome|1-9 / 100 000|Autosomal recessive|Infancy&lt;br&gt;Neonatal|274600 ~</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Deafness autosomal recessive 4; Pendred syndrome</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>600791; 274600</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>7:117199644:ATCT:A</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CFTR</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>rs113993960</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>exonic,nonframeshift deletion</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>(4) practice guideline</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>7105</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>48|Congenital bilateral agenesis of vas deferens&lt;br&gt;Congenital bilateral aplasia of vas deferens|1-5 / 10 000|X-linked recessive&lt;br&gt;or&amp;nbsp;Autosomal recessive|Adolescent&lt;br&gt;Adult|277180 300985 ~586|CF&lt;br&gt;Mucoviscidosis|1-9 / 100 000|Autosomal recessive|All ages|219700 ~60033|-|-|-|-|211400 613021 613071 ~676|-|1-9 / 1 000 000|Autosomal dominant|Childhood&lt;br&gt;Adolescent|167800 ~</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Cystic fibrosis</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>219700</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>11:17496515:C:T</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ABCC8</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>rs764349043</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Conflicting interpretations of pathogenicity</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>(1) criteria provided, conflicting interpretations</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1677653</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>99886|TNDM|Unknown|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;Not applicable|Antenatal&lt;br&gt;Neonatal|601410 610374 610582 ~79134|Developmental delay-epilepsy-neonatal diabetes syndrome|&lt;1 / 1 000 000|Not applicable&lt;br&gt;or&amp;nbsp;Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Infancy&lt;br&gt;Neonatal|606176 ~99885|Monogenic diabetes of infancy&lt;br&gt;PNDM|1-9 / 1 000 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Antenatal&lt;br&gt;Neonatal&lt;br&gt;Infancy|606176 ~276575|Autosomal dominant hyperinsulinemic hypoglycemia due to SUR1 deficiency|Unknown|Autosomal dominant|Infancy&lt;br&gt;Neonatal|256450 ~276598|Hyperinsulinemic hypoglycemia due to SUR1 deficiency, diazoxide-resistant focal form|Unknown|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive|Infancy&lt;br&gt;Neonatal|256450 ~79643|Autosomal recessive hyperinsulinemic hypoglycemia due to SUR1 deficiency|-|Autosomal recessive|-|256450 ~</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Diabetes mellitus, permanent neonatal 3</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>618857</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>12:103306572:A:C</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PAH</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>rs199475598</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>exonic,nonsynonymous SNV</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Likely pathogenic</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pathogenic/Likely pathogenic</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>(2) criteria provided, multiple submitters, no conflicts</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>92734</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2209|Hyperphenylalaninemic embryopathy&lt;br&gt;Maternal PKU&lt;br&gt;Maternal hyperphenylalaninemia&lt;br&gt;Phenylketonuric embryopathy|Unknown|Autosomal recessive|Neonatal&lt;br&gt;Antenatal|261600 ~716|PAH deficiency&lt;br&gt;PKU&lt;br&gt;Phenylalanine hydroxylase deficiency|1-5 / 10 000|Autosomal recessive|Infancy|261600 ~</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Phenylketonuria</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>261600</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>15:91304138:GA:G</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BLM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>rs772495493</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>exonic,frameshift deletion</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Uncertain significance</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>(2) criteria provided, multiple submitters, no conflicts</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>374315</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>125|BSyn|Unknown|Autosomal recessive|Neonatal&lt;br&gt;Antenatal|210900 ~</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Bloom syndrome</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>210900</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>X:25031367:C:A</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ARX</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>het</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>exonic,stopgain</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Pathogenic</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>94083|Partington-Mulley syndrome&lt;br&gt;X-linked intellectual disability-dystonia-dysarthria syndrome|&lt;1 / 1 000 000|X-linked recessive|Childhood|309510 ~1934|EIEE&lt;br&gt;Early infantile epileptic encephalopathy with suppression-bursts&lt;br&gt;Ohtahara syndrome|Unknown|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive&lt;br&gt;or&amp;nbsp;Not applicable|Neonatal|300672 308350 609304 612164 613402 613721 615473 616341 ~3175|-|&lt;1 / 1 000 000|X-linked recessive|No data available|308350 ~3451|Infantile spasms&lt;br&gt;Intellectual disability-hypsarrhythmia syndrome|1-9 / 100 000|Autosomal dominant&lt;br&gt;or&amp;nbsp;Autosomal recessive&lt;br&gt;or&amp;nbsp;X-linked recessive|Infancy&lt;br&gt;Neonatal&lt;br&gt;Childhood|300672 308350 613477 613722 615006 616139 616341 617065 ~364063|-|-|X-linked recessive|Infancy&lt;br&gt;Neonatal|308350 ~777|X-linked non-specific intellectual disability|Unknown|X-linked recessive|Childhood|300046 300047 300062 300114 300115 300143 300210 300271 300324 300355 300372 300387 300419 300428 300433 300436 300454 300498 300504 300505 300518 300558 300705 300716 300802 300803 300844 300848 300849 300850 300851 300852 300919 300928 300978 300983 300984 309530 309549 ~452|X-linked lissencephaly with ambiguous genitalia&lt;br&gt;X-linked lissencephaly-agenesis of the corpus callosum-genital anomalies syndrome&lt;br&gt;XLAG (X-linked lissencephaly with abnormal genitalia) syndrome|Unknown|X-linked recessive|Neonatal|300215 ~2508|Proud-Levine-Carpenter syndrome|Unknown|X-linked recessive|Infancy&lt;br&gt;Neonatal|300004 ~</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Developmental and epileptic encephalopathy 1 (DEE1)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>308350</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>